<commit_message>
fix bug file configurazione e dimesione pannelli
</commit_message>
<xml_diff>
--- a/FileConfigurazione/CDB.xlsx
+++ b/FileConfigurazione/CDB.xlsx
@@ -62,9 +62,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -345,15 +346,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W17"/>
+  <dimension ref="A1:X17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>13301</v>
       </c>
@@ -415,7 +416,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>13302</v>
       </c>
@@ -426,7 +427,7 @@
         <v>15302</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10301</v>
       </c>
@@ -467,7 +468,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10302</v>
       </c>
@@ -484,7 +485,7 @@
         <v>11013</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>12010</v>
       </c>
@@ -552,7 +553,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>12013</v>
       </c>
@@ -620,12 +621,12 @@
         <v>429</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>12303</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E14">
         <v>16027</v>
       </c>
@@ -635,20 +636,20 @@
       <c r="G14">
         <v>16017</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>17301</v>
       </c>
-      <c r="U14">
+      <c r="V14">
         <v>17015</v>
       </c>
-      <c r="V14">
+      <c r="W14">
         <v>17017</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <v>17019</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>16020</v>
       </c>
@@ -671,52 +672,55 @@
         <v>16015</v>
       </c>
       <c r="I15">
+        <v>16014</v>
+      </c>
+      <c r="J15">
         <v>16013</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>440</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>442</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>444</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>446</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>448</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>17010</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>17011</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>17012</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>17013</v>
       </c>
-      <c r="S15">
+      <c r="T15">
         <v>17014</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>17302</v>
       </c>
-      <c r="U15">
+      <c r="V15">
         <v>17016</v>
       </c>
-      <c r="V15">
+      <c r="W15">
         <v>17018</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <v>17020</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>16024</v>
       </c>
@@ -734,63 +738,66 @@
       <c r="H16">
         <v>16012</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="2">
+        <v>16011</v>
+      </c>
+      <c r="J16">
         <v>16010</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>441</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>443</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>445</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>447</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>449</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>17030</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>17031</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>17032</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>17033</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>17034</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>17303</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <v>17036</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <v>17038</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <v>17040</v>
       </c>
     </row>
-    <row r="17" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T17">
+    <row r="17" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U17">
         <v>17304</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <v>17035</v>
       </c>
-      <c r="V17">
+      <c r="W17">
         <v>17037</v>
       </c>
-      <c r="W17">
+      <c r="X17">
         <v>17039</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix bug add script for simulate train
</commit_message>
<xml_diff>
--- a/FileConfigurazione/CDB.xlsx
+++ b/FileConfigurazione/CDB.xlsx
@@ -9,23 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20910" windowHeight="7890"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="9270"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="CDB" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -34,23 +29,315 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -58,17 +345,204 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Colore 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Calcolo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cella collegata" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Cella da controllare" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Colore 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Colore 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Colore 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Colore 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Colore 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Colore 6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Neutrale" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Testo avviso" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Testo descrittivo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titolo" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titolo 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titolo 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titolo 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titolo 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Totale" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Valore non valido" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Valore valido" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -349,7 +823,7 @@
   <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,6 +887,9 @@
         <v>15011</v>
       </c>
       <c r="T1">
+        <v>15010</v>
+      </c>
+      <c r="U1">
         <v>503</v>
       </c>
     </row>
@@ -495,61 +972,61 @@
       <c r="C9">
         <v>12012</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>12301</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>12026</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>12025</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>12024</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>400</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>402</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>404</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>406</v>
       </c>
-      <c r="L9">
+      <c r="N9">
         <v>408</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <v>410</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>412</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>414</v>
       </c>
-      <c r="P9">
+      <c r="R9">
         <v>416</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <v>418</v>
       </c>
-      <c r="R9">
+      <c r="T9">
         <v>420</v>
       </c>
-      <c r="S9">
+      <c r="U9">
         <v>422</v>
       </c>
-      <c r="T9">
+      <c r="V9">
         <v>424</v>
       </c>
-      <c r="U9">
+      <c r="W9">
         <v>426</v>
       </c>
-      <c r="V9">
+      <c r="X9">
         <v>428</v>
       </c>
     </row>
@@ -564,65 +1041,71 @@
         <v>12015</v>
       </c>
       <c r="D10">
+        <v>12016</v>
+      </c>
+      <c r="E10">
         <v>12302</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>12023</v>
       </c>
-      <c r="F10">
+      <c r="G10">
+        <v>12022</v>
+      </c>
+      <c r="H10">
         <v>12021</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>12020</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>401</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>403</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>405</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>407</v>
       </c>
-      <c r="L10">
+      <c r="N10">
         <v>409</v>
       </c>
-      <c r="M10">
+      <c r="O10">
         <v>411</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <v>413</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <v>415</v>
       </c>
-      <c r="P10">
+      <c r="R10">
         <v>417</v>
       </c>
-      <c r="Q10">
+      <c r="S10">
         <v>419</v>
       </c>
-      <c r="R10">
+      <c r="T10">
         <v>421</v>
       </c>
-      <c r="S10">
+      <c r="U10">
         <v>423</v>
       </c>
-      <c r="T10">
+      <c r="V10">
         <v>425</v>
       </c>
-      <c r="U10">
+      <c r="W10">
         <v>427</v>
       </c>
-      <c r="V10">
+      <c r="X10">
         <v>429</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D11">
+      <c r="E11">
         <v>12303</v>
       </c>
     </row>
@@ -730,15 +1213,13 @@
       <c r="D16">
         <v>16026</v>
       </c>
-      <c r="E16" s="1"/>
       <c r="F16">
         <v>16301</v>
       </c>
-      <c r="G16" s="1"/>
       <c r="H16">
         <v>16012</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16">
         <v>16011</v>
       </c>
       <c r="J16">

</xml_diff>